<commit_message>
Fixing small error in Sharing spaces BAU
</commit_message>
<xml_diff>
--- a/Files for shocks/Full scale/m2pc_Full.xlsx
+++ b/Files for shocks/Full scale/m2pc_Full.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/14a790445df90286/Documenti/GitHub/FULFILL_MARIO/Files for shocks/Full scale/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="72" documentId="13_ncr:1_{BD32D5DE-C4F4-41C1-9559-9E2C619F0F48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{41CEA05E-AE60-4DDF-8F10-B310B5E0AC60}"/>
+  <xr:revisionPtr revIDLastSave="75" documentId="13_ncr:1_{BD32D5DE-C4F4-41C1-9559-9E2C619F0F48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{34699579-4310-4EAE-B58C-AF09F4432047}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="m2pc 0 - starting point" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -1232,8 +1232,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8D641CB-B8F7-F548-83F9-F07EC0F19C6D}">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8:G9"/>
+    <sheetView zoomScale="280" zoomScaleNormal="280" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4:G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1464,8 +1464,8 @@
   </sheetPr>
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView tabSelected="1" zoomScale="280" zoomScaleNormal="280" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1544,24 +1544,24 @@
         <v>27</v>
       </c>
       <c r="C4" s="8">
-        <f>C3</f>
-        <v>54.261045846803263</v>
+        <f>'m2pc S - starting point'!C4</f>
+        <v>54.57631730869673</v>
       </c>
       <c r="D4" s="8">
-        <f t="shared" ref="D4:G4" si="0">D3</f>
-        <v>41.725351832173402</v>
+        <f>'m2pc S - starting point'!D4</f>
+        <v>41.927519710129786</v>
       </c>
       <c r="E4" s="8">
-        <f t="shared" si="0"/>
-        <v>45.50824427817038</v>
+        <f>'m2pc S - starting point'!E4</f>
+        <v>45.726043705082326</v>
       </c>
       <c r="F4" s="8">
-        <f t="shared" si="0"/>
-        <v>41.53798146111923</v>
+        <f>'m2pc S - starting point'!F4</f>
+        <v>41.829085437994316</v>
       </c>
       <c r="G4" s="8">
-        <f t="shared" si="0"/>
-        <v>29.429221995017024</v>
+        <f>'m2pc S - starting point'!G4</f>
+        <v>29.648583588236484</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -1572,24 +1572,24 @@
         <v>27</v>
       </c>
       <c r="C5" s="8">
-        <f t="shared" ref="C5:C9" si="1">C4</f>
-        <v>54.261045846803263</v>
+        <f>'m2pc S - starting point'!C5</f>
+        <v>54.785373757055282</v>
       </c>
       <c r="D5" s="8">
-        <f t="shared" ref="D5:D9" si="2">D4</f>
-        <v>41.725351832173402</v>
+        <f>'m2pc S - starting point'!D5</f>
+        <v>42.192433810656532</v>
       </c>
       <c r="E5" s="8">
-        <f t="shared" ref="E5:E9" si="3">E4</f>
-        <v>45.50824427817038</v>
+        <f>'m2pc S - starting point'!E5</f>
+        <v>45.838503973465578</v>
       </c>
       <c r="F5" s="8">
-        <f t="shared" ref="F5:F9" si="4">F4</f>
-        <v>41.53798146111923</v>
+        <f>'m2pc S - starting point'!F5</f>
+        <v>42.135429695368295</v>
       </c>
       <c r="G5" s="8">
-        <f t="shared" ref="G5:G9" si="5">G4</f>
-        <v>29.429221995017024</v>
+        <f>'m2pc S - starting point'!G5</f>
+        <v>29.875666259745085</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -1600,24 +1600,24 @@
         <v>27</v>
       </c>
       <c r="C6" s="8">
-        <f t="shared" si="1"/>
-        <v>54.261045846803263</v>
+        <f>'m2pc S - starting point'!C6</f>
+        <v>54.904229949075301</v>
       </c>
       <c r="D6" s="8">
-        <f t="shared" si="2"/>
-        <v>41.725351832173402</v>
+        <f>'m2pc S - starting point'!D6</f>
+        <v>42.367330988735318</v>
       </c>
       <c r="E6" s="8">
-        <f t="shared" si="3"/>
-        <v>45.50824427817038</v>
+        <f>'m2pc S - starting point'!E6</f>
+        <v>45.880252257058039</v>
       </c>
       <c r="F6" s="8">
-        <f t="shared" si="4"/>
-        <v>41.53798146111923</v>
+        <f>'m2pc S - starting point'!F6</f>
+        <v>42.460431885472488</v>
       </c>
       <c r="G6" s="8">
-        <f t="shared" si="5"/>
-        <v>29.429221995017024</v>
+        <f>'m2pc S - starting point'!G6</f>
+        <v>30.011577235384596</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -1628,24 +1628,24 @@
         <v>27</v>
       </c>
       <c r="C7" s="8">
-        <f t="shared" si="1"/>
-        <v>54.261045846803263</v>
+        <f>'m2pc S - starting point'!C7</f>
+        <v>54.768653239877651</v>
       </c>
       <c r="D7" s="8">
-        <f t="shared" si="2"/>
-        <v>41.725351832173402</v>
+        <f>'m2pc S - starting point'!D7</f>
+        <v>42.238805652368626</v>
       </c>
       <c r="E7" s="8">
-        <f t="shared" si="3"/>
-        <v>45.50824427817038</v>
+        <f>'m2pc S - starting point'!E7</f>
+        <v>45.804424212825189</v>
       </c>
       <c r="F7" s="8">
-        <f t="shared" si="4"/>
-        <v>41.53798146111923</v>
+        <f>'m2pc S - starting point'!F7</f>
+        <v>42.602175551555199</v>
       </c>
       <c r="G7" s="8">
-        <f t="shared" si="5"/>
-        <v>29.429221995017024</v>
+        <f>'m2pc S - starting point'!G7</f>
+        <v>30.094200856988813</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
@@ -1656,24 +1656,24 @@
         <v>27</v>
       </c>
       <c r="C8" s="8">
-        <f t="shared" si="1"/>
-        <v>54.261045846803263</v>
+        <f>'m2pc S - starting point'!C8</f>
+        <v>54.219729023162785</v>
       </c>
       <c r="D8" s="8">
-        <f t="shared" si="2"/>
-        <v>41.725351832173402</v>
+        <f>'m2pc S - starting point'!D8</f>
+        <v>41.88202984670388</v>
       </c>
       <c r="E8" s="8">
-        <f t="shared" si="3"/>
-        <v>45.50824427817038</v>
+        <f>'m2pc S - starting point'!E8</f>
+        <v>45.418860130202006</v>
       </c>
       <c r="F8" s="8">
-        <f t="shared" si="4"/>
-        <v>41.53798146111923</v>
+        <f>'m2pc S - starting point'!F8</f>
+        <v>42.331809530047231</v>
       </c>
       <c r="G8" s="8">
-        <f t="shared" si="5"/>
-        <v>29.429221995017024</v>
+        <f>'m2pc S - starting point'!G8</f>
+        <v>29.998060769980995</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
@@ -1684,24 +1684,24 @@
         <v>27</v>
       </c>
       <c r="C9" s="8">
-        <f t="shared" si="1"/>
-        <v>54.261045846803263</v>
+        <f>'m2pc S - starting point'!C9</f>
+        <v>52.796572524038808</v>
       </c>
       <c r="D9" s="8">
-        <f t="shared" si="2"/>
-        <v>41.725351832173402</v>
+        <f>'m2pc S - starting point'!D9</f>
+        <v>41.158125442575255</v>
       </c>
       <c r="E9" s="8">
-        <f t="shared" si="3"/>
-        <v>45.50824427817038</v>
+        <f>'m2pc S - starting point'!E9</f>
+        <v>44.551093593831069</v>
       </c>
       <c r="F9" s="8">
-        <f t="shared" si="4"/>
-        <v>41.53798146111923</v>
+        <f>'m2pc S - starting point'!F9</f>
+        <v>41.369009232557275</v>
       </c>
       <c r="G9" s="8">
-        <f t="shared" si="5"/>
-        <v>29.429221995017024</v>
+        <f>'m2pc S - starting point'!G9</f>
+        <v>29.598359919879897</v>
       </c>
     </row>
   </sheetData>
@@ -1714,7 +1714,7 @@
   <dimension ref="A1:AC12"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="J1" sqref="J1:J1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2865,7 +2865,7 @@
   <dimension ref="A1:AC12"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H41" sqref="H41"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4013,7 +4013,7 @@
   <dimension ref="A1:AC10"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="AC10" sqref="AC10"/>
+      <selection activeCell="J1" sqref="J1:J1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5160,8 +5160,8 @@
   </sheetPr>
   <dimension ref="A1:AC10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5609,111 +5609,111 @@
       </c>
       <c r="C5" s="6" cm="1">
         <f t="array" ref="C5">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('m2pc BAU-S - starting point'!$C$2:$G$9,('m2pc BAU-S - starting point'!$A$2:$A$9='m2pc BAU-S'!$A5)),'m2pc BAU-S - starting point'!$C$1:$G$1='m2pc BAU-S'!C$1),'m2pc BAU-S - starting point'!$B$2='m2pc BAU-S'!$B5)),0)</f>
-        <v>45.50824427817038</v>
+        <v>45.726043705082326</v>
       </c>
       <c r="D5" s="6" cm="1">
         <f t="array" ref="D5">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('m2pc BAU-S - starting point'!$C$2:$G$9,('m2pc BAU-S - starting point'!$A$2:$A$9='m2pc BAU-S'!$A5)),'m2pc BAU-S - starting point'!$C$1:$G$1='m2pc BAU-S'!D$1),'m2pc BAU-S - starting point'!$B$2='m2pc BAU-S'!$B5)),0)</f>
-        <v>41.725351832173402</v>
+        <v>41.927519710129786</v>
       </c>
       <c r="E5" s="6" cm="1">
         <f t="array" ref="E5">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('m2pc BAU-S - starting point'!$C$2:$G$9,('m2pc BAU-S - starting point'!$A$2:$A$9='m2pc BAU-S'!$A5)),'m2pc BAU-S - starting point'!$C$1:$G$1='m2pc BAU-S'!E$1),'m2pc BAU-S - starting point'!$B$2='m2pc BAU-S'!$B5)),0)</f>
-        <v>29.429221995017024</v>
+        <v>29.648583588236484</v>
       </c>
       <c r="F5" s="6" cm="1">
         <f t="array" ref="F5">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('m2pc BAU-S - starting point'!$C$2:$G$9,('m2pc BAU-S - starting point'!$A$2:$A$9='m2pc BAU-S'!$A5)),'m2pc BAU-S - starting point'!$C$1:$G$1='m2pc BAU-S'!F$1),'m2pc BAU-S - starting point'!$B$2='m2pc BAU-S'!$B5)),0)</f>
-        <v>29.429221995017024</v>
+        <v>29.648583588236484</v>
       </c>
       <c r="G5" s="6" cm="1">
         <f t="array" ref="G5">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('m2pc BAU-S - starting point'!$C$2:$G$9,('m2pc BAU-S - starting point'!$A$2:$A$9='m2pc BAU-S'!$A5)),'m2pc BAU-S - starting point'!$C$1:$G$1='m2pc BAU-S'!G$1),'m2pc BAU-S - starting point'!$B$2='m2pc BAU-S'!$B5)),0)</f>
-        <v>54.261045846803263</v>
+        <v>54.57631730869673</v>
       </c>
       <c r="H5" s="6" cm="1">
         <f t="array" ref="H5">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('m2pc BAU-S - starting point'!$C$2:$G$9,('m2pc BAU-S - starting point'!$A$2:$A$9='m2pc BAU-S'!$A5)),'m2pc BAU-S - starting point'!$C$1:$G$1='m2pc BAU-S'!H$1),'m2pc BAU-S - starting point'!$B$2='m2pc BAU-S'!$B5)),0)</f>
-        <v>41.53798146111923</v>
+        <v>41.829085437994316</v>
       </c>
       <c r="I5" s="6" cm="1">
         <f t="array" ref="I5">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('m2pc BAU-S - starting point'!$C$2:$G$9,('m2pc BAU-S - starting point'!$A$2:$A$9='m2pc BAU-S'!$A5)),'m2pc BAU-S - starting point'!$C$1:$G$1='m2pc BAU-S'!I$1),'m2pc BAU-S - starting point'!$B$2='m2pc BAU-S'!$B5)),0)</f>
-        <v>54.261045846803263</v>
+        <v>54.57631730869673</v>
       </c>
       <c r="J5" s="6" cm="1">
         <f t="array" ref="J5">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('m2pc BAU-S - starting point'!$C$2:$G$9,('m2pc BAU-S - starting point'!$A$2:$A$9='m2pc BAU-S'!$A5)),'m2pc BAU-S - starting point'!$C$1:$G$1='m2pc BAU-S'!J$1),'m2pc BAU-S - starting point'!$B$2='m2pc BAU-S'!$B5)),0)</f>
-        <v>41.53798146111923</v>
+        <v>41.829085437994316</v>
       </c>
       <c r="K5" s="6" cm="1">
         <f t="array" ref="K5">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('m2pc BAU-S - starting point'!$C$2:$G$9,('m2pc BAU-S - starting point'!$A$2:$A$9='m2pc BAU-S'!$A5)),'m2pc BAU-S - starting point'!$C$1:$G$1='m2pc BAU-S'!K$1),'m2pc BAU-S - starting point'!$B$2='m2pc BAU-S'!$B5)),0)</f>
-        <v>41.725351832173402</v>
+        <v>41.927519710129786</v>
       </c>
       <c r="L5" s="6" cm="1">
         <f t="array" ref="L5">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('m2pc BAU-S - starting point'!$C$2:$G$9,('m2pc BAU-S - starting point'!$A$2:$A$9='m2pc BAU-S'!$A5)),'m2pc BAU-S - starting point'!$C$1:$G$1='m2pc BAU-S'!L$1),'m2pc BAU-S - starting point'!$B$2='m2pc BAU-S'!$B5)),0)</f>
-        <v>41.725351832173402</v>
+        <v>41.927519710129786</v>
       </c>
       <c r="M5" s="6" cm="1">
         <f t="array" ref="M5">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('m2pc BAU-S - starting point'!$C$2:$G$9,('m2pc BAU-S - starting point'!$A$2:$A$9='m2pc BAU-S'!$A5)),'m2pc BAU-S - starting point'!$C$1:$G$1='m2pc BAU-S'!M$1),'m2pc BAU-S - starting point'!$B$2='m2pc BAU-S'!$B5)),0)</f>
-        <v>45.50824427817038</v>
+        <v>45.726043705082326</v>
       </c>
       <c r="N5" s="6" cm="1">
         <f t="array" ref="N5">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('m2pc BAU-S - starting point'!$C$2:$G$9,('m2pc BAU-S - starting point'!$A$2:$A$9='m2pc BAU-S'!$A5)),'m2pc BAU-S - starting point'!$C$1:$G$1='m2pc BAU-S'!N$1),'m2pc BAU-S - starting point'!$B$2='m2pc BAU-S'!$B5)),0)</f>
-        <v>41.53798146111923</v>
+        <v>41.829085437994316</v>
       </c>
       <c r="O5" s="6" cm="1">
         <f t="array" ref="O5">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('m2pc BAU-S - starting point'!$C$2:$G$9,('m2pc BAU-S - starting point'!$A$2:$A$9='m2pc BAU-S'!$A5)),'m2pc BAU-S - starting point'!$C$1:$G$1='m2pc BAU-S'!O$1),'m2pc BAU-S - starting point'!$B$2='m2pc BAU-S'!$B5)),0)</f>
-        <v>41.53798146111923</v>
+        <v>41.829085437994316</v>
       </c>
       <c r="P5" s="6" cm="1">
         <f t="array" ref="P5">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('m2pc BAU-S - starting point'!$C$2:$G$9,('m2pc BAU-S - starting point'!$A$2:$A$9='m2pc BAU-S'!$A5)),'m2pc BAU-S - starting point'!$C$1:$G$1='m2pc BAU-S'!P$1),'m2pc BAU-S - starting point'!$B$2='m2pc BAU-S'!$B5)),0)</f>
-        <v>41.725351832173402</v>
+        <v>41.927519710129786</v>
       </c>
       <c r="Q5" s="6" cm="1">
         <f t="array" ref="Q5">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('m2pc BAU-S - starting point'!$C$2:$G$9,('m2pc BAU-S - starting point'!$A$2:$A$9='m2pc BAU-S'!$A5)),'m2pc BAU-S - starting point'!$C$1:$G$1='m2pc BAU-S'!Q$1),'m2pc BAU-S - starting point'!$B$2='m2pc BAU-S'!$B5)),0)</f>
-        <v>41.53798146111923</v>
+        <v>41.829085437994316</v>
       </c>
       <c r="R5" s="6" cm="1">
         <f t="array" ref="R5">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('m2pc BAU-S - starting point'!$C$2:$G$9,('m2pc BAU-S - starting point'!$A$2:$A$9='m2pc BAU-S'!$A5)),'m2pc BAU-S - starting point'!$C$1:$G$1='m2pc BAU-S'!R$1),'m2pc BAU-S - starting point'!$B$2='m2pc BAU-S'!$B5)),0)</f>
-        <v>29.429221995017024</v>
+        <v>29.648583588236484</v>
       </c>
       <c r="S5" s="6" cm="1">
         <f t="array" ref="S5">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('m2pc BAU-S - starting point'!$C$2:$G$9,('m2pc BAU-S - starting point'!$A$2:$A$9='m2pc BAU-S'!$A5)),'m2pc BAU-S - starting point'!$C$1:$G$1='m2pc BAU-S'!S$1),'m2pc BAU-S - starting point'!$B$2='m2pc BAU-S'!$B5)),0)</f>
-        <v>41.53798146111923</v>
+        <v>41.829085437994316</v>
       </c>
       <c r="T5" s="6" cm="1">
         <f t="array" ref="T5">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('m2pc BAU-S - starting point'!$C$2:$G$9,('m2pc BAU-S - starting point'!$A$2:$A$9='m2pc BAU-S'!$A5)),'m2pc BAU-S - starting point'!$C$1:$G$1='m2pc BAU-S'!T$1),'m2pc BAU-S - starting point'!$B$2='m2pc BAU-S'!$B5)),0)</f>
-        <v>54.261045846803263</v>
+        <v>54.57631730869673</v>
       </c>
       <c r="U5" s="6" cm="1">
         <f t="array" ref="U5">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('m2pc BAU-S - starting point'!$C$2:$G$9,('m2pc BAU-S - starting point'!$A$2:$A$9='m2pc BAU-S'!$A5)),'m2pc BAU-S - starting point'!$C$1:$G$1='m2pc BAU-S'!U$1),'m2pc BAU-S - starting point'!$B$2='m2pc BAU-S'!$B5)),0)</f>
-        <v>54.261045846803263</v>
+        <v>54.57631730869673</v>
       </c>
       <c r="V5" s="6" cm="1">
         <f t="array" ref="V5">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('m2pc BAU-S - starting point'!$C$2:$G$9,('m2pc BAU-S - starting point'!$A$2:$A$9='m2pc BAU-S'!$A5)),'m2pc BAU-S - starting point'!$C$1:$G$1='m2pc BAU-S'!V$1),'m2pc BAU-S - starting point'!$B$2='m2pc BAU-S'!$B5)),0)</f>
-        <v>54.261045846803263</v>
+        <v>54.57631730869673</v>
       </c>
       <c r="W5" s="6" cm="1">
         <f t="array" ref="W5">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('m2pc BAU-S - starting point'!$C$2:$G$9,('m2pc BAU-S - starting point'!$A$2:$A$9='m2pc BAU-S'!$A5)),'m2pc BAU-S - starting point'!$C$1:$G$1='m2pc BAU-S'!W$1),'m2pc BAU-S - starting point'!$B$2='m2pc BAU-S'!$B5)),0)</f>
-        <v>29.429221995017024</v>
+        <v>29.648583588236484</v>
       </c>
       <c r="X5" s="6" cm="1">
         <f t="array" ref="X5">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('m2pc BAU-S - starting point'!$C$2:$G$9,('m2pc BAU-S - starting point'!$A$2:$A$9='m2pc BAU-S'!$A5)),'m2pc BAU-S - starting point'!$C$1:$G$1='m2pc BAU-S'!X$1),'m2pc BAU-S - starting point'!$B$2='m2pc BAU-S'!$B5)),0)</f>
-        <v>45.50824427817038</v>
+        <v>45.726043705082326</v>
       </c>
       <c r="Y5" s="6" cm="1">
         <f t="array" ref="Y5">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('m2pc BAU-S - starting point'!$C$2:$G$9,('m2pc BAU-S - starting point'!$A$2:$A$9='m2pc BAU-S'!$A5)),'m2pc BAU-S - starting point'!$C$1:$G$1='m2pc BAU-S'!Y$1),'m2pc BAU-S - starting point'!$B$2='m2pc BAU-S'!$B5)),0)</f>
-        <v>29.429221995017024</v>
+        <v>29.648583588236484</v>
       </c>
       <c r="Z5" s="6" cm="1">
         <f t="array" ref="Z5">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('m2pc BAU-S - starting point'!$C$2:$G$9,('m2pc BAU-S - starting point'!$A$2:$A$9='m2pc BAU-S'!$A5)),'m2pc BAU-S - starting point'!$C$1:$G$1='m2pc BAU-S'!Z$1),'m2pc BAU-S - starting point'!$B$2='m2pc BAU-S'!$B5)),0)</f>
-        <v>29.429221995017024</v>
+        <v>29.648583588236484</v>
       </c>
       <c r="AA5" s="6" cm="1">
         <f t="array" ref="AA5">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('m2pc BAU-S - starting point'!$C$2:$G$9,('m2pc BAU-S - starting point'!$A$2:$A$9='m2pc BAU-S'!$A5)),'m2pc BAU-S - starting point'!$C$1:$G$1='m2pc BAU-S'!AA$1),'m2pc BAU-S - starting point'!$B$2='m2pc BAU-S'!$B5)),0)</f>
-        <v>41.53798146111923</v>
+        <v>41.829085437994316</v>
       </c>
       <c r="AB5" s="6" cm="1">
         <f t="array" ref="AB5">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('m2pc BAU-S - starting point'!$C$2:$G$9,('m2pc BAU-S - starting point'!$A$2:$A$9='m2pc BAU-S'!$A5)),'m2pc BAU-S - starting point'!$C$1:$G$1='m2pc BAU-S'!AB$1),'m2pc BAU-S - starting point'!$B$2='m2pc BAU-S'!$B5)),0)</f>
-        <v>41.725351832173402</v>
+        <v>41.927519710129786</v>
       </c>
       <c r="AC5" s="6" cm="1">
         <f t="array" ref="AC5">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('m2pc BAU-S - starting point'!$C$2:$G$9,('m2pc BAU-S - starting point'!$A$2:$A$9='m2pc BAU-S'!$A5)),'m2pc BAU-S - starting point'!$C$1:$G$1='m2pc BAU-S'!AC$1),'m2pc BAU-S - starting point'!$B$2='m2pc BAU-S'!$B5)),0)</f>
-        <v>45.50824427817038</v>
+        <v>45.726043705082326</v>
       </c>
     </row>
     <row r="6" spans="1:29" x14ac:dyDescent="0.3">
@@ -5725,111 +5725,111 @@
       </c>
       <c r="C6" s="6" cm="1">
         <f t="array" ref="C6">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('m2pc BAU-S - starting point'!$C$2:$G$9,('m2pc BAU-S - starting point'!$A$2:$A$9='m2pc BAU-S'!$A6)),'m2pc BAU-S - starting point'!$C$1:$G$1='m2pc BAU-S'!C$1),'m2pc BAU-S - starting point'!$B$2='m2pc BAU-S'!$B6)),0)</f>
-        <v>45.50824427817038</v>
+        <v>45.838503973465578</v>
       </c>
       <c r="D6" s="6" cm="1">
         <f t="array" ref="D6">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('m2pc BAU-S - starting point'!$C$2:$G$9,('m2pc BAU-S - starting point'!$A$2:$A$9='m2pc BAU-S'!$A6)),'m2pc BAU-S - starting point'!$C$1:$G$1='m2pc BAU-S'!D$1),'m2pc BAU-S - starting point'!$B$2='m2pc BAU-S'!$B6)),0)</f>
-        <v>41.725351832173402</v>
+        <v>42.192433810656532</v>
       </c>
       <c r="E6" s="6" cm="1">
         <f t="array" ref="E6">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('m2pc BAU-S - starting point'!$C$2:$G$9,('m2pc BAU-S - starting point'!$A$2:$A$9='m2pc BAU-S'!$A6)),'m2pc BAU-S - starting point'!$C$1:$G$1='m2pc BAU-S'!E$1),'m2pc BAU-S - starting point'!$B$2='m2pc BAU-S'!$B6)),0)</f>
-        <v>29.429221995017024</v>
+        <v>29.875666259745085</v>
       </c>
       <c r="F6" s="6" cm="1">
         <f t="array" ref="F6">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('m2pc BAU-S - starting point'!$C$2:$G$9,('m2pc BAU-S - starting point'!$A$2:$A$9='m2pc BAU-S'!$A6)),'m2pc BAU-S - starting point'!$C$1:$G$1='m2pc BAU-S'!F$1),'m2pc BAU-S - starting point'!$B$2='m2pc BAU-S'!$B6)),0)</f>
-        <v>29.429221995017024</v>
+        <v>29.875666259745085</v>
       </c>
       <c r="G6" s="6" cm="1">
         <f t="array" ref="G6">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('m2pc BAU-S - starting point'!$C$2:$G$9,('m2pc BAU-S - starting point'!$A$2:$A$9='m2pc BAU-S'!$A6)),'m2pc BAU-S - starting point'!$C$1:$G$1='m2pc BAU-S'!G$1),'m2pc BAU-S - starting point'!$B$2='m2pc BAU-S'!$B6)),0)</f>
-        <v>54.261045846803263</v>
+        <v>54.785373757055282</v>
       </c>
       <c r="H6" s="6" cm="1">
         <f t="array" ref="H6">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('m2pc BAU-S - starting point'!$C$2:$G$9,('m2pc BAU-S - starting point'!$A$2:$A$9='m2pc BAU-S'!$A6)),'m2pc BAU-S - starting point'!$C$1:$G$1='m2pc BAU-S'!H$1),'m2pc BAU-S - starting point'!$B$2='m2pc BAU-S'!$B6)),0)</f>
-        <v>41.53798146111923</v>
+        <v>42.135429695368295</v>
       </c>
       <c r="I6" s="6" cm="1">
         <f t="array" ref="I6">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('m2pc BAU-S - starting point'!$C$2:$G$9,('m2pc BAU-S - starting point'!$A$2:$A$9='m2pc BAU-S'!$A6)),'m2pc BAU-S - starting point'!$C$1:$G$1='m2pc BAU-S'!I$1),'m2pc BAU-S - starting point'!$B$2='m2pc BAU-S'!$B6)),0)</f>
-        <v>54.261045846803263</v>
+        <v>54.785373757055282</v>
       </c>
       <c r="J6" s="6" cm="1">
         <f t="array" ref="J6">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('m2pc BAU-S - starting point'!$C$2:$G$9,('m2pc BAU-S - starting point'!$A$2:$A$9='m2pc BAU-S'!$A6)),'m2pc BAU-S - starting point'!$C$1:$G$1='m2pc BAU-S'!J$1),'m2pc BAU-S - starting point'!$B$2='m2pc BAU-S'!$B6)),0)</f>
-        <v>41.53798146111923</v>
+        <v>42.135429695368295</v>
       </c>
       <c r="K6" s="6" cm="1">
         <f t="array" ref="K6">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('m2pc BAU-S - starting point'!$C$2:$G$9,('m2pc BAU-S - starting point'!$A$2:$A$9='m2pc BAU-S'!$A6)),'m2pc BAU-S - starting point'!$C$1:$G$1='m2pc BAU-S'!K$1),'m2pc BAU-S - starting point'!$B$2='m2pc BAU-S'!$B6)),0)</f>
-        <v>41.725351832173402</v>
+        <v>42.192433810656532</v>
       </c>
       <c r="L6" s="6" cm="1">
         <f t="array" ref="L6">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('m2pc BAU-S - starting point'!$C$2:$G$9,('m2pc BAU-S - starting point'!$A$2:$A$9='m2pc BAU-S'!$A6)),'m2pc BAU-S - starting point'!$C$1:$G$1='m2pc BAU-S'!L$1),'m2pc BAU-S - starting point'!$B$2='m2pc BAU-S'!$B6)),0)</f>
-        <v>41.725351832173402</v>
+        <v>42.192433810656532</v>
       </c>
       <c r="M6" s="6" cm="1">
         <f t="array" ref="M6">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('m2pc BAU-S - starting point'!$C$2:$G$9,('m2pc BAU-S - starting point'!$A$2:$A$9='m2pc BAU-S'!$A6)),'m2pc BAU-S - starting point'!$C$1:$G$1='m2pc BAU-S'!M$1),'m2pc BAU-S - starting point'!$B$2='m2pc BAU-S'!$B6)),0)</f>
-        <v>45.50824427817038</v>
+        <v>45.838503973465578</v>
       </c>
       <c r="N6" s="6" cm="1">
         <f t="array" ref="N6">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('m2pc BAU-S - starting point'!$C$2:$G$9,('m2pc BAU-S - starting point'!$A$2:$A$9='m2pc BAU-S'!$A6)),'m2pc BAU-S - starting point'!$C$1:$G$1='m2pc BAU-S'!N$1),'m2pc BAU-S - starting point'!$B$2='m2pc BAU-S'!$B6)),0)</f>
-        <v>41.53798146111923</v>
+        <v>42.135429695368295</v>
       </c>
       <c r="O6" s="6" cm="1">
         <f t="array" ref="O6">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('m2pc BAU-S - starting point'!$C$2:$G$9,('m2pc BAU-S - starting point'!$A$2:$A$9='m2pc BAU-S'!$A6)),'m2pc BAU-S - starting point'!$C$1:$G$1='m2pc BAU-S'!O$1),'m2pc BAU-S - starting point'!$B$2='m2pc BAU-S'!$B6)),0)</f>
-        <v>41.53798146111923</v>
+        <v>42.135429695368295</v>
       </c>
       <c r="P6" s="6" cm="1">
         <f t="array" ref="P6">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('m2pc BAU-S - starting point'!$C$2:$G$9,('m2pc BAU-S - starting point'!$A$2:$A$9='m2pc BAU-S'!$A6)),'m2pc BAU-S - starting point'!$C$1:$G$1='m2pc BAU-S'!P$1),'m2pc BAU-S - starting point'!$B$2='m2pc BAU-S'!$B6)),0)</f>
-        <v>41.725351832173402</v>
+        <v>42.192433810656532</v>
       </c>
       <c r="Q6" s="6" cm="1">
         <f t="array" ref="Q6">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('m2pc BAU-S - starting point'!$C$2:$G$9,('m2pc BAU-S - starting point'!$A$2:$A$9='m2pc BAU-S'!$A6)),'m2pc BAU-S - starting point'!$C$1:$G$1='m2pc BAU-S'!Q$1),'m2pc BAU-S - starting point'!$B$2='m2pc BAU-S'!$B6)),0)</f>
-        <v>41.53798146111923</v>
+        <v>42.135429695368295</v>
       </c>
       <c r="R6" s="6" cm="1">
         <f t="array" ref="R6">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('m2pc BAU-S - starting point'!$C$2:$G$9,('m2pc BAU-S - starting point'!$A$2:$A$9='m2pc BAU-S'!$A6)),'m2pc BAU-S - starting point'!$C$1:$G$1='m2pc BAU-S'!R$1),'m2pc BAU-S - starting point'!$B$2='m2pc BAU-S'!$B6)),0)</f>
-        <v>29.429221995017024</v>
+        <v>29.875666259745085</v>
       </c>
       <c r="S6" s="6" cm="1">
         <f t="array" ref="S6">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('m2pc BAU-S - starting point'!$C$2:$G$9,('m2pc BAU-S - starting point'!$A$2:$A$9='m2pc BAU-S'!$A6)),'m2pc BAU-S - starting point'!$C$1:$G$1='m2pc BAU-S'!S$1),'m2pc BAU-S - starting point'!$B$2='m2pc BAU-S'!$B6)),0)</f>
-        <v>41.53798146111923</v>
+        <v>42.135429695368295</v>
       </c>
       <c r="T6" s="6" cm="1">
         <f t="array" ref="T6">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('m2pc BAU-S - starting point'!$C$2:$G$9,('m2pc BAU-S - starting point'!$A$2:$A$9='m2pc BAU-S'!$A6)),'m2pc BAU-S - starting point'!$C$1:$G$1='m2pc BAU-S'!T$1),'m2pc BAU-S - starting point'!$B$2='m2pc BAU-S'!$B6)),0)</f>
-        <v>54.261045846803263</v>
+        <v>54.785373757055282</v>
       </c>
       <c r="U6" s="6" cm="1">
         <f t="array" ref="U6">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('m2pc BAU-S - starting point'!$C$2:$G$9,('m2pc BAU-S - starting point'!$A$2:$A$9='m2pc BAU-S'!$A6)),'m2pc BAU-S - starting point'!$C$1:$G$1='m2pc BAU-S'!U$1),'m2pc BAU-S - starting point'!$B$2='m2pc BAU-S'!$B6)),0)</f>
-        <v>54.261045846803263</v>
+        <v>54.785373757055282</v>
       </c>
       <c r="V6" s="6" cm="1">
         <f t="array" ref="V6">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('m2pc BAU-S - starting point'!$C$2:$G$9,('m2pc BAU-S - starting point'!$A$2:$A$9='m2pc BAU-S'!$A6)),'m2pc BAU-S - starting point'!$C$1:$G$1='m2pc BAU-S'!V$1),'m2pc BAU-S - starting point'!$B$2='m2pc BAU-S'!$B6)),0)</f>
-        <v>54.261045846803263</v>
+        <v>54.785373757055282</v>
       </c>
       <c r="W6" s="6" cm="1">
         <f t="array" ref="W6">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('m2pc BAU-S - starting point'!$C$2:$G$9,('m2pc BAU-S - starting point'!$A$2:$A$9='m2pc BAU-S'!$A6)),'m2pc BAU-S - starting point'!$C$1:$G$1='m2pc BAU-S'!W$1),'m2pc BAU-S - starting point'!$B$2='m2pc BAU-S'!$B6)),0)</f>
-        <v>29.429221995017024</v>
+        <v>29.875666259745085</v>
       </c>
       <c r="X6" s="6" cm="1">
         <f t="array" ref="X6">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('m2pc BAU-S - starting point'!$C$2:$G$9,('m2pc BAU-S - starting point'!$A$2:$A$9='m2pc BAU-S'!$A6)),'m2pc BAU-S - starting point'!$C$1:$G$1='m2pc BAU-S'!X$1),'m2pc BAU-S - starting point'!$B$2='m2pc BAU-S'!$B6)),0)</f>
-        <v>45.50824427817038</v>
+        <v>45.838503973465578</v>
       </c>
       <c r="Y6" s="6" cm="1">
         <f t="array" ref="Y6">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('m2pc BAU-S - starting point'!$C$2:$G$9,('m2pc BAU-S - starting point'!$A$2:$A$9='m2pc BAU-S'!$A6)),'m2pc BAU-S - starting point'!$C$1:$G$1='m2pc BAU-S'!Y$1),'m2pc BAU-S - starting point'!$B$2='m2pc BAU-S'!$B6)),0)</f>
-        <v>29.429221995017024</v>
+        <v>29.875666259745085</v>
       </c>
       <c r="Z6" s="6" cm="1">
         <f t="array" ref="Z6">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('m2pc BAU-S - starting point'!$C$2:$G$9,('m2pc BAU-S - starting point'!$A$2:$A$9='m2pc BAU-S'!$A6)),'m2pc BAU-S - starting point'!$C$1:$G$1='m2pc BAU-S'!Z$1),'m2pc BAU-S - starting point'!$B$2='m2pc BAU-S'!$B6)),0)</f>
-        <v>29.429221995017024</v>
+        <v>29.875666259745085</v>
       </c>
       <c r="AA6" s="6" cm="1">
         <f t="array" ref="AA6">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('m2pc BAU-S - starting point'!$C$2:$G$9,('m2pc BAU-S - starting point'!$A$2:$A$9='m2pc BAU-S'!$A6)),'m2pc BAU-S - starting point'!$C$1:$G$1='m2pc BAU-S'!AA$1),'m2pc BAU-S - starting point'!$B$2='m2pc BAU-S'!$B6)),0)</f>
-        <v>41.53798146111923</v>
+        <v>42.135429695368295</v>
       </c>
       <c r="AB6" s="6" cm="1">
         <f t="array" ref="AB6">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('m2pc BAU-S - starting point'!$C$2:$G$9,('m2pc BAU-S - starting point'!$A$2:$A$9='m2pc BAU-S'!$A6)),'m2pc BAU-S - starting point'!$C$1:$G$1='m2pc BAU-S'!AB$1),'m2pc BAU-S - starting point'!$B$2='m2pc BAU-S'!$B6)),0)</f>
-        <v>41.725351832173402</v>
+        <v>42.192433810656532</v>
       </c>
       <c r="AC6" s="6" cm="1">
         <f t="array" ref="AC6">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('m2pc BAU-S - starting point'!$C$2:$G$9,('m2pc BAU-S - starting point'!$A$2:$A$9='m2pc BAU-S'!$A6)),'m2pc BAU-S - starting point'!$C$1:$G$1='m2pc BAU-S'!AC$1),'m2pc BAU-S - starting point'!$B$2='m2pc BAU-S'!$B6)),0)</f>
-        <v>45.50824427817038</v>
+        <v>45.838503973465578</v>
       </c>
     </row>
     <row r="7" spans="1:29" x14ac:dyDescent="0.3">
@@ -5841,111 +5841,111 @@
       </c>
       <c r="C7" s="6" cm="1">
         <f t="array" ref="C7">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('m2pc BAU-S - starting point'!$C$2:$G$9,('m2pc BAU-S - starting point'!$A$2:$A$9='m2pc BAU-S'!$A7)),'m2pc BAU-S - starting point'!$C$1:$G$1='m2pc BAU-S'!C$1),'m2pc BAU-S - starting point'!$B$2='m2pc BAU-S'!$B7)),0)</f>
-        <v>45.50824427817038</v>
+        <v>45.880252257058039</v>
       </c>
       <c r="D7" s="6" cm="1">
         <f t="array" ref="D7">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('m2pc BAU-S - starting point'!$C$2:$G$9,('m2pc BAU-S - starting point'!$A$2:$A$9='m2pc BAU-S'!$A7)),'m2pc BAU-S - starting point'!$C$1:$G$1='m2pc BAU-S'!D$1),'m2pc BAU-S - starting point'!$B$2='m2pc BAU-S'!$B7)),0)</f>
-        <v>41.725351832173402</v>
+        <v>42.367330988735318</v>
       </c>
       <c r="E7" s="6" cm="1">
         <f t="array" ref="E7">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('m2pc BAU-S - starting point'!$C$2:$G$9,('m2pc BAU-S - starting point'!$A$2:$A$9='m2pc BAU-S'!$A7)),'m2pc BAU-S - starting point'!$C$1:$G$1='m2pc BAU-S'!E$1),'m2pc BAU-S - starting point'!$B$2='m2pc BAU-S'!$B7)),0)</f>
-        <v>29.429221995017024</v>
+        <v>30.011577235384596</v>
       </c>
       <c r="F7" s="6" cm="1">
         <f t="array" ref="F7">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('m2pc BAU-S - starting point'!$C$2:$G$9,('m2pc BAU-S - starting point'!$A$2:$A$9='m2pc BAU-S'!$A7)),'m2pc BAU-S - starting point'!$C$1:$G$1='m2pc BAU-S'!F$1),'m2pc BAU-S - starting point'!$B$2='m2pc BAU-S'!$B7)),0)</f>
-        <v>29.429221995017024</v>
+        <v>30.011577235384596</v>
       </c>
       <c r="G7" s="6" cm="1">
         <f t="array" ref="G7">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('m2pc BAU-S - starting point'!$C$2:$G$9,('m2pc BAU-S - starting point'!$A$2:$A$9='m2pc BAU-S'!$A7)),'m2pc BAU-S - starting point'!$C$1:$G$1='m2pc BAU-S'!G$1),'m2pc BAU-S - starting point'!$B$2='m2pc BAU-S'!$B7)),0)</f>
-        <v>54.261045846803263</v>
+        <v>54.904229949075301</v>
       </c>
       <c r="H7" s="6" cm="1">
         <f t="array" ref="H7">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('m2pc BAU-S - starting point'!$C$2:$G$9,('m2pc BAU-S - starting point'!$A$2:$A$9='m2pc BAU-S'!$A7)),'m2pc BAU-S - starting point'!$C$1:$G$1='m2pc BAU-S'!H$1),'m2pc BAU-S - starting point'!$B$2='m2pc BAU-S'!$B7)),0)</f>
-        <v>41.53798146111923</v>
+        <v>42.460431885472488</v>
       </c>
       <c r="I7" s="6" cm="1">
         <f t="array" ref="I7">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('m2pc BAU-S - starting point'!$C$2:$G$9,('m2pc BAU-S - starting point'!$A$2:$A$9='m2pc BAU-S'!$A7)),'m2pc BAU-S - starting point'!$C$1:$G$1='m2pc BAU-S'!I$1),'m2pc BAU-S - starting point'!$B$2='m2pc BAU-S'!$B7)),0)</f>
-        <v>54.261045846803263</v>
+        <v>54.904229949075301</v>
       </c>
       <c r="J7" s="6" cm="1">
         <f t="array" ref="J7">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('m2pc BAU-S - starting point'!$C$2:$G$9,('m2pc BAU-S - starting point'!$A$2:$A$9='m2pc BAU-S'!$A7)),'m2pc BAU-S - starting point'!$C$1:$G$1='m2pc BAU-S'!J$1),'m2pc BAU-S - starting point'!$B$2='m2pc BAU-S'!$B7)),0)</f>
-        <v>41.53798146111923</v>
+        <v>42.460431885472488</v>
       </c>
       <c r="K7" s="6" cm="1">
         <f t="array" ref="K7">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('m2pc BAU-S - starting point'!$C$2:$G$9,('m2pc BAU-S - starting point'!$A$2:$A$9='m2pc BAU-S'!$A7)),'m2pc BAU-S - starting point'!$C$1:$G$1='m2pc BAU-S'!K$1),'m2pc BAU-S - starting point'!$B$2='m2pc BAU-S'!$B7)),0)</f>
-        <v>41.725351832173402</v>
+        <v>42.367330988735318</v>
       </c>
       <c r="L7" s="6" cm="1">
         <f t="array" ref="L7">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('m2pc BAU-S - starting point'!$C$2:$G$9,('m2pc BAU-S - starting point'!$A$2:$A$9='m2pc BAU-S'!$A7)),'m2pc BAU-S - starting point'!$C$1:$G$1='m2pc BAU-S'!L$1),'m2pc BAU-S - starting point'!$B$2='m2pc BAU-S'!$B7)),0)</f>
-        <v>41.725351832173402</v>
+        <v>42.367330988735318</v>
       </c>
       <c r="M7" s="6" cm="1">
         <f t="array" ref="M7">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('m2pc BAU-S - starting point'!$C$2:$G$9,('m2pc BAU-S - starting point'!$A$2:$A$9='m2pc BAU-S'!$A7)),'m2pc BAU-S - starting point'!$C$1:$G$1='m2pc BAU-S'!M$1),'m2pc BAU-S - starting point'!$B$2='m2pc BAU-S'!$B7)),0)</f>
-        <v>45.50824427817038</v>
+        <v>45.880252257058039</v>
       </c>
       <c r="N7" s="6" cm="1">
         <f t="array" ref="N7">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('m2pc BAU-S - starting point'!$C$2:$G$9,('m2pc BAU-S - starting point'!$A$2:$A$9='m2pc BAU-S'!$A7)),'m2pc BAU-S - starting point'!$C$1:$G$1='m2pc BAU-S'!N$1),'m2pc BAU-S - starting point'!$B$2='m2pc BAU-S'!$B7)),0)</f>
-        <v>41.53798146111923</v>
+        <v>42.460431885472488</v>
       </c>
       <c r="O7" s="6" cm="1">
         <f t="array" ref="O7">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('m2pc BAU-S - starting point'!$C$2:$G$9,('m2pc BAU-S - starting point'!$A$2:$A$9='m2pc BAU-S'!$A7)),'m2pc BAU-S - starting point'!$C$1:$G$1='m2pc BAU-S'!O$1),'m2pc BAU-S - starting point'!$B$2='m2pc BAU-S'!$B7)),0)</f>
-        <v>41.53798146111923</v>
+        <v>42.460431885472488</v>
       </c>
       <c r="P7" s="6" cm="1">
         <f t="array" ref="P7">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('m2pc BAU-S - starting point'!$C$2:$G$9,('m2pc BAU-S - starting point'!$A$2:$A$9='m2pc BAU-S'!$A7)),'m2pc BAU-S - starting point'!$C$1:$G$1='m2pc BAU-S'!P$1),'m2pc BAU-S - starting point'!$B$2='m2pc BAU-S'!$B7)),0)</f>
-        <v>41.725351832173402</v>
+        <v>42.367330988735318</v>
       </c>
       <c r="Q7" s="6" cm="1">
         <f t="array" ref="Q7">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('m2pc BAU-S - starting point'!$C$2:$G$9,('m2pc BAU-S - starting point'!$A$2:$A$9='m2pc BAU-S'!$A7)),'m2pc BAU-S - starting point'!$C$1:$G$1='m2pc BAU-S'!Q$1),'m2pc BAU-S - starting point'!$B$2='m2pc BAU-S'!$B7)),0)</f>
-        <v>41.53798146111923</v>
+        <v>42.460431885472488</v>
       </c>
       <c r="R7" s="6" cm="1">
         <f t="array" ref="R7">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('m2pc BAU-S - starting point'!$C$2:$G$9,('m2pc BAU-S - starting point'!$A$2:$A$9='m2pc BAU-S'!$A7)),'m2pc BAU-S - starting point'!$C$1:$G$1='m2pc BAU-S'!R$1),'m2pc BAU-S - starting point'!$B$2='m2pc BAU-S'!$B7)),0)</f>
-        <v>29.429221995017024</v>
+        <v>30.011577235384596</v>
       </c>
       <c r="S7" s="6" cm="1">
         <f t="array" ref="S7">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('m2pc BAU-S - starting point'!$C$2:$G$9,('m2pc BAU-S - starting point'!$A$2:$A$9='m2pc BAU-S'!$A7)),'m2pc BAU-S - starting point'!$C$1:$G$1='m2pc BAU-S'!S$1),'m2pc BAU-S - starting point'!$B$2='m2pc BAU-S'!$B7)),0)</f>
-        <v>41.53798146111923</v>
+        <v>42.460431885472488</v>
       </c>
       <c r="T7" s="6" cm="1">
         <f t="array" ref="T7">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('m2pc BAU-S - starting point'!$C$2:$G$9,('m2pc BAU-S - starting point'!$A$2:$A$9='m2pc BAU-S'!$A7)),'m2pc BAU-S - starting point'!$C$1:$G$1='m2pc BAU-S'!T$1),'m2pc BAU-S - starting point'!$B$2='m2pc BAU-S'!$B7)),0)</f>
-        <v>54.261045846803263</v>
+        <v>54.904229949075301</v>
       </c>
       <c r="U7" s="6" cm="1">
         <f t="array" ref="U7">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('m2pc BAU-S - starting point'!$C$2:$G$9,('m2pc BAU-S - starting point'!$A$2:$A$9='m2pc BAU-S'!$A7)),'m2pc BAU-S - starting point'!$C$1:$G$1='m2pc BAU-S'!U$1),'m2pc BAU-S - starting point'!$B$2='m2pc BAU-S'!$B7)),0)</f>
-        <v>54.261045846803263</v>
+        <v>54.904229949075301</v>
       </c>
       <c r="V7" s="6" cm="1">
         <f t="array" ref="V7">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('m2pc BAU-S - starting point'!$C$2:$G$9,('m2pc BAU-S - starting point'!$A$2:$A$9='m2pc BAU-S'!$A7)),'m2pc BAU-S - starting point'!$C$1:$G$1='m2pc BAU-S'!V$1),'m2pc BAU-S - starting point'!$B$2='m2pc BAU-S'!$B7)),0)</f>
-        <v>54.261045846803263</v>
+        <v>54.904229949075301</v>
       </c>
       <c r="W7" s="6" cm="1">
         <f t="array" ref="W7">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('m2pc BAU-S - starting point'!$C$2:$G$9,('m2pc BAU-S - starting point'!$A$2:$A$9='m2pc BAU-S'!$A7)),'m2pc BAU-S - starting point'!$C$1:$G$1='m2pc BAU-S'!W$1),'m2pc BAU-S - starting point'!$B$2='m2pc BAU-S'!$B7)),0)</f>
-        <v>29.429221995017024</v>
+        <v>30.011577235384596</v>
       </c>
       <c r="X7" s="6" cm="1">
         <f t="array" ref="X7">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('m2pc BAU-S - starting point'!$C$2:$G$9,('m2pc BAU-S - starting point'!$A$2:$A$9='m2pc BAU-S'!$A7)),'m2pc BAU-S - starting point'!$C$1:$G$1='m2pc BAU-S'!X$1),'m2pc BAU-S - starting point'!$B$2='m2pc BAU-S'!$B7)),0)</f>
-        <v>45.50824427817038</v>
+        <v>45.880252257058039</v>
       </c>
       <c r="Y7" s="6" cm="1">
         <f t="array" ref="Y7">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('m2pc BAU-S - starting point'!$C$2:$G$9,('m2pc BAU-S - starting point'!$A$2:$A$9='m2pc BAU-S'!$A7)),'m2pc BAU-S - starting point'!$C$1:$G$1='m2pc BAU-S'!Y$1),'m2pc BAU-S - starting point'!$B$2='m2pc BAU-S'!$B7)),0)</f>
-        <v>29.429221995017024</v>
+        <v>30.011577235384596</v>
       </c>
       <c r="Z7" s="6" cm="1">
         <f t="array" ref="Z7">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('m2pc BAU-S - starting point'!$C$2:$G$9,('m2pc BAU-S - starting point'!$A$2:$A$9='m2pc BAU-S'!$A7)),'m2pc BAU-S - starting point'!$C$1:$G$1='m2pc BAU-S'!Z$1),'m2pc BAU-S - starting point'!$B$2='m2pc BAU-S'!$B7)),0)</f>
-        <v>29.429221995017024</v>
+        <v>30.011577235384596</v>
       </c>
       <c r="AA7" s="6" cm="1">
         <f t="array" ref="AA7">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('m2pc BAU-S - starting point'!$C$2:$G$9,('m2pc BAU-S - starting point'!$A$2:$A$9='m2pc BAU-S'!$A7)),'m2pc BAU-S - starting point'!$C$1:$G$1='m2pc BAU-S'!AA$1),'m2pc BAU-S - starting point'!$B$2='m2pc BAU-S'!$B7)),0)</f>
-        <v>41.53798146111923</v>
+        <v>42.460431885472488</v>
       </c>
       <c r="AB7" s="6" cm="1">
         <f t="array" ref="AB7">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('m2pc BAU-S - starting point'!$C$2:$G$9,('m2pc BAU-S - starting point'!$A$2:$A$9='m2pc BAU-S'!$A7)),'m2pc BAU-S - starting point'!$C$1:$G$1='m2pc BAU-S'!AB$1),'m2pc BAU-S - starting point'!$B$2='m2pc BAU-S'!$B7)),0)</f>
-        <v>41.725351832173402</v>
+        <v>42.367330988735318</v>
       </c>
       <c r="AC7" s="6" cm="1">
         <f t="array" ref="AC7">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('m2pc BAU-S - starting point'!$C$2:$G$9,('m2pc BAU-S - starting point'!$A$2:$A$9='m2pc BAU-S'!$A7)),'m2pc BAU-S - starting point'!$C$1:$G$1='m2pc BAU-S'!AC$1),'m2pc BAU-S - starting point'!$B$2='m2pc BAU-S'!$B7)),0)</f>
-        <v>45.50824427817038</v>
+        <v>45.880252257058039</v>
       </c>
     </row>
     <row r="8" spans="1:29" x14ac:dyDescent="0.3">
@@ -5957,111 +5957,111 @@
       </c>
       <c r="C8" s="6" cm="1">
         <f t="array" ref="C8">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('m2pc BAU-S - starting point'!$C$2:$G$9,('m2pc BAU-S - starting point'!$A$2:$A$9='m2pc BAU-S'!$A8)),'m2pc BAU-S - starting point'!$C$1:$G$1='m2pc BAU-S'!C$1),'m2pc BAU-S - starting point'!$B$2='m2pc BAU-S'!$B8)),0)</f>
-        <v>45.50824427817038</v>
+        <v>45.804424212825189</v>
       </c>
       <c r="D8" s="6" cm="1">
         <f t="array" ref="D8">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('m2pc BAU-S - starting point'!$C$2:$G$9,('m2pc BAU-S - starting point'!$A$2:$A$9='m2pc BAU-S'!$A8)),'m2pc BAU-S - starting point'!$C$1:$G$1='m2pc BAU-S'!D$1),'m2pc BAU-S - starting point'!$B$2='m2pc BAU-S'!$B8)),0)</f>
-        <v>41.725351832173402</v>
+        <v>42.238805652368626</v>
       </c>
       <c r="E8" s="6" cm="1">
         <f t="array" ref="E8">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('m2pc BAU-S - starting point'!$C$2:$G$9,('m2pc BAU-S - starting point'!$A$2:$A$9='m2pc BAU-S'!$A8)),'m2pc BAU-S - starting point'!$C$1:$G$1='m2pc BAU-S'!E$1),'m2pc BAU-S - starting point'!$B$2='m2pc BAU-S'!$B8)),0)</f>
-        <v>29.429221995017024</v>
+        <v>30.094200856988813</v>
       </c>
       <c r="F8" s="6" cm="1">
         <f t="array" ref="F8">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('m2pc BAU-S - starting point'!$C$2:$G$9,('m2pc BAU-S - starting point'!$A$2:$A$9='m2pc BAU-S'!$A8)),'m2pc BAU-S - starting point'!$C$1:$G$1='m2pc BAU-S'!F$1),'m2pc BAU-S - starting point'!$B$2='m2pc BAU-S'!$B8)),0)</f>
-        <v>29.429221995017024</v>
+        <v>30.094200856988813</v>
       </c>
       <c r="G8" s="6" cm="1">
         <f t="array" ref="G8">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('m2pc BAU-S - starting point'!$C$2:$G$9,('m2pc BAU-S - starting point'!$A$2:$A$9='m2pc BAU-S'!$A8)),'m2pc BAU-S - starting point'!$C$1:$G$1='m2pc BAU-S'!G$1),'m2pc BAU-S - starting point'!$B$2='m2pc BAU-S'!$B8)),0)</f>
-        <v>54.261045846803263</v>
+        <v>54.768653239877651</v>
       </c>
       <c r="H8" s="6" cm="1">
         <f t="array" ref="H8">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('m2pc BAU-S - starting point'!$C$2:$G$9,('m2pc BAU-S - starting point'!$A$2:$A$9='m2pc BAU-S'!$A8)),'m2pc BAU-S - starting point'!$C$1:$G$1='m2pc BAU-S'!H$1),'m2pc BAU-S - starting point'!$B$2='m2pc BAU-S'!$B8)),0)</f>
-        <v>41.53798146111923</v>
+        <v>42.602175551555199</v>
       </c>
       <c r="I8" s="6" cm="1">
         <f t="array" ref="I8">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('m2pc BAU-S - starting point'!$C$2:$G$9,('m2pc BAU-S - starting point'!$A$2:$A$9='m2pc BAU-S'!$A8)),'m2pc BAU-S - starting point'!$C$1:$G$1='m2pc BAU-S'!I$1),'m2pc BAU-S - starting point'!$B$2='m2pc BAU-S'!$B8)),0)</f>
-        <v>54.261045846803263</v>
+        <v>54.768653239877651</v>
       </c>
       <c r="J8" s="6" cm="1">
         <f t="array" ref="J8">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('m2pc BAU-S - starting point'!$C$2:$G$9,('m2pc BAU-S - starting point'!$A$2:$A$9='m2pc BAU-S'!$A8)),'m2pc BAU-S - starting point'!$C$1:$G$1='m2pc BAU-S'!J$1),'m2pc BAU-S - starting point'!$B$2='m2pc BAU-S'!$B8)),0)</f>
-        <v>41.53798146111923</v>
+        <v>42.602175551555199</v>
       </c>
       <c r="K8" s="6" cm="1">
         <f t="array" ref="K8">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('m2pc BAU-S - starting point'!$C$2:$G$9,('m2pc BAU-S - starting point'!$A$2:$A$9='m2pc BAU-S'!$A8)),'m2pc BAU-S - starting point'!$C$1:$G$1='m2pc BAU-S'!K$1),'m2pc BAU-S - starting point'!$B$2='m2pc BAU-S'!$B8)),0)</f>
-        <v>41.725351832173402</v>
+        <v>42.238805652368626</v>
       </c>
       <c r="L8" s="6" cm="1">
         <f t="array" ref="L8">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('m2pc BAU-S - starting point'!$C$2:$G$9,('m2pc BAU-S - starting point'!$A$2:$A$9='m2pc BAU-S'!$A8)),'m2pc BAU-S - starting point'!$C$1:$G$1='m2pc BAU-S'!L$1),'m2pc BAU-S - starting point'!$B$2='m2pc BAU-S'!$B8)),0)</f>
-        <v>41.725351832173402</v>
+        <v>42.238805652368626</v>
       </c>
       <c r="M8" s="6" cm="1">
         <f t="array" ref="M8">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('m2pc BAU-S - starting point'!$C$2:$G$9,('m2pc BAU-S - starting point'!$A$2:$A$9='m2pc BAU-S'!$A8)),'m2pc BAU-S - starting point'!$C$1:$G$1='m2pc BAU-S'!M$1),'m2pc BAU-S - starting point'!$B$2='m2pc BAU-S'!$B8)),0)</f>
-        <v>45.50824427817038</v>
+        <v>45.804424212825189</v>
       </c>
       <c r="N8" s="6" cm="1">
         <f t="array" ref="N8">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('m2pc BAU-S - starting point'!$C$2:$G$9,('m2pc BAU-S - starting point'!$A$2:$A$9='m2pc BAU-S'!$A8)),'m2pc BAU-S - starting point'!$C$1:$G$1='m2pc BAU-S'!N$1),'m2pc BAU-S - starting point'!$B$2='m2pc BAU-S'!$B8)),0)</f>
-        <v>41.53798146111923</v>
+        <v>42.602175551555199</v>
       </c>
       <c r="O8" s="6" cm="1">
         <f t="array" ref="O8">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('m2pc BAU-S - starting point'!$C$2:$G$9,('m2pc BAU-S - starting point'!$A$2:$A$9='m2pc BAU-S'!$A8)),'m2pc BAU-S - starting point'!$C$1:$G$1='m2pc BAU-S'!O$1),'m2pc BAU-S - starting point'!$B$2='m2pc BAU-S'!$B8)),0)</f>
-        <v>41.53798146111923</v>
+        <v>42.602175551555199</v>
       </c>
       <c r="P8" s="6" cm="1">
         <f t="array" ref="P8">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('m2pc BAU-S - starting point'!$C$2:$G$9,('m2pc BAU-S - starting point'!$A$2:$A$9='m2pc BAU-S'!$A8)),'m2pc BAU-S - starting point'!$C$1:$G$1='m2pc BAU-S'!P$1),'m2pc BAU-S - starting point'!$B$2='m2pc BAU-S'!$B8)),0)</f>
-        <v>41.725351832173402</v>
+        <v>42.238805652368626</v>
       </c>
       <c r="Q8" s="6" cm="1">
         <f t="array" ref="Q8">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('m2pc BAU-S - starting point'!$C$2:$G$9,('m2pc BAU-S - starting point'!$A$2:$A$9='m2pc BAU-S'!$A8)),'m2pc BAU-S - starting point'!$C$1:$G$1='m2pc BAU-S'!Q$1),'m2pc BAU-S - starting point'!$B$2='m2pc BAU-S'!$B8)),0)</f>
-        <v>41.53798146111923</v>
+        <v>42.602175551555199</v>
       </c>
       <c r="R8" s="6" cm="1">
         <f t="array" ref="R8">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('m2pc BAU-S - starting point'!$C$2:$G$9,('m2pc BAU-S - starting point'!$A$2:$A$9='m2pc BAU-S'!$A8)),'m2pc BAU-S - starting point'!$C$1:$G$1='m2pc BAU-S'!R$1),'m2pc BAU-S - starting point'!$B$2='m2pc BAU-S'!$B8)),0)</f>
-        <v>29.429221995017024</v>
+        <v>30.094200856988813</v>
       </c>
       <c r="S8" s="6" cm="1">
         <f t="array" ref="S8">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('m2pc BAU-S - starting point'!$C$2:$G$9,('m2pc BAU-S - starting point'!$A$2:$A$9='m2pc BAU-S'!$A8)),'m2pc BAU-S - starting point'!$C$1:$G$1='m2pc BAU-S'!S$1),'m2pc BAU-S - starting point'!$B$2='m2pc BAU-S'!$B8)),0)</f>
-        <v>41.53798146111923</v>
+        <v>42.602175551555199</v>
       </c>
       <c r="T8" s="6" cm="1">
         <f t="array" ref="T8">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('m2pc BAU-S - starting point'!$C$2:$G$9,('m2pc BAU-S - starting point'!$A$2:$A$9='m2pc BAU-S'!$A8)),'m2pc BAU-S - starting point'!$C$1:$G$1='m2pc BAU-S'!T$1),'m2pc BAU-S - starting point'!$B$2='m2pc BAU-S'!$B8)),0)</f>
-        <v>54.261045846803263</v>
+        <v>54.768653239877651</v>
       </c>
       <c r="U8" s="6" cm="1">
         <f t="array" ref="U8">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('m2pc BAU-S - starting point'!$C$2:$G$9,('m2pc BAU-S - starting point'!$A$2:$A$9='m2pc BAU-S'!$A8)),'m2pc BAU-S - starting point'!$C$1:$G$1='m2pc BAU-S'!U$1),'m2pc BAU-S - starting point'!$B$2='m2pc BAU-S'!$B8)),0)</f>
-        <v>54.261045846803263</v>
+        <v>54.768653239877651</v>
       </c>
       <c r="V8" s="6" cm="1">
         <f t="array" ref="V8">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('m2pc BAU-S - starting point'!$C$2:$G$9,('m2pc BAU-S - starting point'!$A$2:$A$9='m2pc BAU-S'!$A8)),'m2pc BAU-S - starting point'!$C$1:$G$1='m2pc BAU-S'!V$1),'m2pc BAU-S - starting point'!$B$2='m2pc BAU-S'!$B8)),0)</f>
-        <v>54.261045846803263</v>
+        <v>54.768653239877651</v>
       </c>
       <c r="W8" s="6" cm="1">
         <f t="array" ref="W8">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('m2pc BAU-S - starting point'!$C$2:$G$9,('m2pc BAU-S - starting point'!$A$2:$A$9='m2pc BAU-S'!$A8)),'m2pc BAU-S - starting point'!$C$1:$G$1='m2pc BAU-S'!W$1),'m2pc BAU-S - starting point'!$B$2='m2pc BAU-S'!$B8)),0)</f>
-        <v>29.429221995017024</v>
+        <v>30.094200856988813</v>
       </c>
       <c r="X8" s="6" cm="1">
         <f t="array" ref="X8">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('m2pc BAU-S - starting point'!$C$2:$G$9,('m2pc BAU-S - starting point'!$A$2:$A$9='m2pc BAU-S'!$A8)),'m2pc BAU-S - starting point'!$C$1:$G$1='m2pc BAU-S'!X$1),'m2pc BAU-S - starting point'!$B$2='m2pc BAU-S'!$B8)),0)</f>
-        <v>45.50824427817038</v>
+        <v>45.804424212825189</v>
       </c>
       <c r="Y8" s="6" cm="1">
         <f t="array" ref="Y8">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('m2pc BAU-S - starting point'!$C$2:$G$9,('m2pc BAU-S - starting point'!$A$2:$A$9='m2pc BAU-S'!$A8)),'m2pc BAU-S - starting point'!$C$1:$G$1='m2pc BAU-S'!Y$1),'m2pc BAU-S - starting point'!$B$2='m2pc BAU-S'!$B8)),0)</f>
-        <v>29.429221995017024</v>
+        <v>30.094200856988813</v>
       </c>
       <c r="Z8" s="6" cm="1">
         <f t="array" ref="Z8">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('m2pc BAU-S - starting point'!$C$2:$G$9,('m2pc BAU-S - starting point'!$A$2:$A$9='m2pc BAU-S'!$A8)),'m2pc BAU-S - starting point'!$C$1:$G$1='m2pc BAU-S'!Z$1),'m2pc BAU-S - starting point'!$B$2='m2pc BAU-S'!$B8)),0)</f>
-        <v>29.429221995017024</v>
+        <v>30.094200856988813</v>
       </c>
       <c r="AA8" s="6" cm="1">
         <f t="array" ref="AA8">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('m2pc BAU-S - starting point'!$C$2:$G$9,('m2pc BAU-S - starting point'!$A$2:$A$9='m2pc BAU-S'!$A8)),'m2pc BAU-S - starting point'!$C$1:$G$1='m2pc BAU-S'!AA$1),'m2pc BAU-S - starting point'!$B$2='m2pc BAU-S'!$B8)),0)</f>
-        <v>41.53798146111923</v>
+        <v>42.602175551555199</v>
       </c>
       <c r="AB8" s="6" cm="1">
         <f t="array" ref="AB8">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('m2pc BAU-S - starting point'!$C$2:$G$9,('m2pc BAU-S - starting point'!$A$2:$A$9='m2pc BAU-S'!$A8)),'m2pc BAU-S - starting point'!$C$1:$G$1='m2pc BAU-S'!AB$1),'m2pc BAU-S - starting point'!$B$2='m2pc BAU-S'!$B8)),0)</f>
-        <v>41.725351832173402</v>
+        <v>42.238805652368626</v>
       </c>
       <c r="AC8" s="6" cm="1">
         <f t="array" ref="AC8">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('m2pc BAU-S - starting point'!$C$2:$G$9,('m2pc BAU-S - starting point'!$A$2:$A$9='m2pc BAU-S'!$A8)),'m2pc BAU-S - starting point'!$C$1:$G$1='m2pc BAU-S'!AC$1),'m2pc BAU-S - starting point'!$B$2='m2pc BAU-S'!$B8)),0)</f>
-        <v>45.50824427817038</v>
+        <v>45.804424212825189</v>
       </c>
     </row>
     <row r="9" spans="1:29" x14ac:dyDescent="0.3">
@@ -6073,111 +6073,111 @@
       </c>
       <c r="C9" s="6" cm="1">
         <f t="array" ref="C9">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('m2pc BAU-S - starting point'!$C$2:$G$9,('m2pc BAU-S - starting point'!$A$2:$A$9='m2pc BAU-S'!$A9)),'m2pc BAU-S - starting point'!$C$1:$G$1='m2pc BAU-S'!C$1),'m2pc BAU-S - starting point'!$B$2='m2pc BAU-S'!$B9)),0)</f>
-        <v>45.50824427817038</v>
+        <v>45.418860130202006</v>
       </c>
       <c r="D9" s="6" cm="1">
         <f t="array" ref="D9">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('m2pc BAU-S - starting point'!$C$2:$G$9,('m2pc BAU-S - starting point'!$A$2:$A$9='m2pc BAU-S'!$A9)),'m2pc BAU-S - starting point'!$C$1:$G$1='m2pc BAU-S'!D$1),'m2pc BAU-S - starting point'!$B$2='m2pc BAU-S'!$B9)),0)</f>
-        <v>41.725351832173402</v>
+        <v>41.88202984670388</v>
       </c>
       <c r="E9" s="6" cm="1">
         <f t="array" ref="E9">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('m2pc BAU-S - starting point'!$C$2:$G$9,('m2pc BAU-S - starting point'!$A$2:$A$9='m2pc BAU-S'!$A9)),'m2pc BAU-S - starting point'!$C$1:$G$1='m2pc BAU-S'!E$1),'m2pc BAU-S - starting point'!$B$2='m2pc BAU-S'!$B9)),0)</f>
-        <v>29.429221995017024</v>
+        <v>29.998060769980995</v>
       </c>
       <c r="F9" s="6" cm="1">
         <f t="array" ref="F9">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('m2pc BAU-S - starting point'!$C$2:$G$9,('m2pc BAU-S - starting point'!$A$2:$A$9='m2pc BAU-S'!$A9)),'m2pc BAU-S - starting point'!$C$1:$G$1='m2pc BAU-S'!F$1),'m2pc BAU-S - starting point'!$B$2='m2pc BAU-S'!$B9)),0)</f>
-        <v>29.429221995017024</v>
+        <v>29.998060769980995</v>
       </c>
       <c r="G9" s="6" cm="1">
         <f t="array" ref="G9">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('m2pc BAU-S - starting point'!$C$2:$G$9,('m2pc BAU-S - starting point'!$A$2:$A$9='m2pc BAU-S'!$A9)),'m2pc BAU-S - starting point'!$C$1:$G$1='m2pc BAU-S'!G$1),'m2pc BAU-S - starting point'!$B$2='m2pc BAU-S'!$B9)),0)</f>
-        <v>54.261045846803263</v>
+        <v>54.219729023162785</v>
       </c>
       <c r="H9" s="6" cm="1">
         <f t="array" ref="H9">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('m2pc BAU-S - starting point'!$C$2:$G$9,('m2pc BAU-S - starting point'!$A$2:$A$9='m2pc BAU-S'!$A9)),'m2pc BAU-S - starting point'!$C$1:$G$1='m2pc BAU-S'!H$1),'m2pc BAU-S - starting point'!$B$2='m2pc BAU-S'!$B9)),0)</f>
-        <v>41.53798146111923</v>
+        <v>42.331809530047231</v>
       </c>
       <c r="I9" s="6" cm="1">
         <f t="array" ref="I9">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('m2pc BAU-S - starting point'!$C$2:$G$9,('m2pc BAU-S - starting point'!$A$2:$A$9='m2pc BAU-S'!$A9)),'m2pc BAU-S - starting point'!$C$1:$G$1='m2pc BAU-S'!I$1),'m2pc BAU-S - starting point'!$B$2='m2pc BAU-S'!$B9)),0)</f>
-        <v>54.261045846803263</v>
+        <v>54.219729023162785</v>
       </c>
       <c r="J9" s="6" cm="1">
         <f t="array" ref="J9">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('m2pc BAU-S - starting point'!$C$2:$G$9,('m2pc BAU-S - starting point'!$A$2:$A$9='m2pc BAU-S'!$A9)),'m2pc BAU-S - starting point'!$C$1:$G$1='m2pc BAU-S'!J$1),'m2pc BAU-S - starting point'!$B$2='m2pc BAU-S'!$B9)),0)</f>
-        <v>41.53798146111923</v>
+        <v>42.331809530047231</v>
       </c>
       <c r="K9" s="6" cm="1">
         <f t="array" ref="K9">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('m2pc BAU-S - starting point'!$C$2:$G$9,('m2pc BAU-S - starting point'!$A$2:$A$9='m2pc BAU-S'!$A9)),'m2pc BAU-S - starting point'!$C$1:$G$1='m2pc BAU-S'!K$1),'m2pc BAU-S - starting point'!$B$2='m2pc BAU-S'!$B9)),0)</f>
-        <v>41.725351832173402</v>
+        <v>41.88202984670388</v>
       </c>
       <c r="L9" s="6" cm="1">
         <f t="array" ref="L9">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('m2pc BAU-S - starting point'!$C$2:$G$9,('m2pc BAU-S - starting point'!$A$2:$A$9='m2pc BAU-S'!$A9)),'m2pc BAU-S - starting point'!$C$1:$G$1='m2pc BAU-S'!L$1),'m2pc BAU-S - starting point'!$B$2='m2pc BAU-S'!$B9)),0)</f>
-        <v>41.725351832173402</v>
+        <v>41.88202984670388</v>
       </c>
       <c r="M9" s="6" cm="1">
         <f t="array" ref="M9">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('m2pc BAU-S - starting point'!$C$2:$G$9,('m2pc BAU-S - starting point'!$A$2:$A$9='m2pc BAU-S'!$A9)),'m2pc BAU-S - starting point'!$C$1:$G$1='m2pc BAU-S'!M$1),'m2pc BAU-S - starting point'!$B$2='m2pc BAU-S'!$B9)),0)</f>
-        <v>45.50824427817038</v>
+        <v>45.418860130202006</v>
       </c>
       <c r="N9" s="6" cm="1">
         <f t="array" ref="N9">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('m2pc BAU-S - starting point'!$C$2:$G$9,('m2pc BAU-S - starting point'!$A$2:$A$9='m2pc BAU-S'!$A9)),'m2pc BAU-S - starting point'!$C$1:$G$1='m2pc BAU-S'!N$1),'m2pc BAU-S - starting point'!$B$2='m2pc BAU-S'!$B9)),0)</f>
-        <v>41.53798146111923</v>
+        <v>42.331809530047231</v>
       </c>
       <c r="O9" s="6" cm="1">
         <f t="array" ref="O9">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('m2pc BAU-S - starting point'!$C$2:$G$9,('m2pc BAU-S - starting point'!$A$2:$A$9='m2pc BAU-S'!$A9)),'m2pc BAU-S - starting point'!$C$1:$G$1='m2pc BAU-S'!O$1),'m2pc BAU-S - starting point'!$B$2='m2pc BAU-S'!$B9)),0)</f>
-        <v>41.53798146111923</v>
+        <v>42.331809530047231</v>
       </c>
       <c r="P9" s="6" cm="1">
         <f t="array" ref="P9">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('m2pc BAU-S - starting point'!$C$2:$G$9,('m2pc BAU-S - starting point'!$A$2:$A$9='m2pc BAU-S'!$A9)),'m2pc BAU-S - starting point'!$C$1:$G$1='m2pc BAU-S'!P$1),'m2pc BAU-S - starting point'!$B$2='m2pc BAU-S'!$B9)),0)</f>
-        <v>41.725351832173402</v>
+        <v>41.88202984670388</v>
       </c>
       <c r="Q9" s="6" cm="1">
         <f t="array" ref="Q9">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('m2pc BAU-S - starting point'!$C$2:$G$9,('m2pc BAU-S - starting point'!$A$2:$A$9='m2pc BAU-S'!$A9)),'m2pc BAU-S - starting point'!$C$1:$G$1='m2pc BAU-S'!Q$1),'m2pc BAU-S - starting point'!$B$2='m2pc BAU-S'!$B9)),0)</f>
-        <v>41.53798146111923</v>
+        <v>42.331809530047231</v>
       </c>
       <c r="R9" s="6" cm="1">
         <f t="array" ref="R9">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('m2pc BAU-S - starting point'!$C$2:$G$9,('m2pc BAU-S - starting point'!$A$2:$A$9='m2pc BAU-S'!$A9)),'m2pc BAU-S - starting point'!$C$1:$G$1='m2pc BAU-S'!R$1),'m2pc BAU-S - starting point'!$B$2='m2pc BAU-S'!$B9)),0)</f>
-        <v>29.429221995017024</v>
+        <v>29.998060769980995</v>
       </c>
       <c r="S9" s="6" cm="1">
         <f t="array" ref="S9">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('m2pc BAU-S - starting point'!$C$2:$G$9,('m2pc BAU-S - starting point'!$A$2:$A$9='m2pc BAU-S'!$A9)),'m2pc BAU-S - starting point'!$C$1:$G$1='m2pc BAU-S'!S$1),'m2pc BAU-S - starting point'!$B$2='m2pc BAU-S'!$B9)),0)</f>
-        <v>41.53798146111923</v>
+        <v>42.331809530047231</v>
       </c>
       <c r="T9" s="6" cm="1">
         <f t="array" ref="T9">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('m2pc BAU-S - starting point'!$C$2:$G$9,('m2pc BAU-S - starting point'!$A$2:$A$9='m2pc BAU-S'!$A9)),'m2pc BAU-S - starting point'!$C$1:$G$1='m2pc BAU-S'!T$1),'m2pc BAU-S - starting point'!$B$2='m2pc BAU-S'!$B9)),0)</f>
-        <v>54.261045846803263</v>
+        <v>54.219729023162785</v>
       </c>
       <c r="U9" s="6" cm="1">
         <f t="array" ref="U9">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('m2pc BAU-S - starting point'!$C$2:$G$9,('m2pc BAU-S - starting point'!$A$2:$A$9='m2pc BAU-S'!$A9)),'m2pc BAU-S - starting point'!$C$1:$G$1='m2pc BAU-S'!U$1),'m2pc BAU-S - starting point'!$B$2='m2pc BAU-S'!$B9)),0)</f>
-        <v>54.261045846803263</v>
+        <v>54.219729023162785</v>
       </c>
       <c r="V9" s="6" cm="1">
         <f t="array" ref="V9">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('m2pc BAU-S - starting point'!$C$2:$G$9,('m2pc BAU-S - starting point'!$A$2:$A$9='m2pc BAU-S'!$A9)),'m2pc BAU-S - starting point'!$C$1:$G$1='m2pc BAU-S'!V$1),'m2pc BAU-S - starting point'!$B$2='m2pc BAU-S'!$B9)),0)</f>
-        <v>54.261045846803263</v>
+        <v>54.219729023162785</v>
       </c>
       <c r="W9" s="6" cm="1">
         <f t="array" ref="W9">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('m2pc BAU-S - starting point'!$C$2:$G$9,('m2pc BAU-S - starting point'!$A$2:$A$9='m2pc BAU-S'!$A9)),'m2pc BAU-S - starting point'!$C$1:$G$1='m2pc BAU-S'!W$1),'m2pc BAU-S - starting point'!$B$2='m2pc BAU-S'!$B9)),0)</f>
-        <v>29.429221995017024</v>
+        <v>29.998060769980995</v>
       </c>
       <c r="X9" s="6" cm="1">
         <f t="array" ref="X9">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('m2pc BAU-S - starting point'!$C$2:$G$9,('m2pc BAU-S - starting point'!$A$2:$A$9='m2pc BAU-S'!$A9)),'m2pc BAU-S - starting point'!$C$1:$G$1='m2pc BAU-S'!X$1),'m2pc BAU-S - starting point'!$B$2='m2pc BAU-S'!$B9)),0)</f>
-        <v>45.50824427817038</v>
+        <v>45.418860130202006</v>
       </c>
       <c r="Y9" s="6" cm="1">
         <f t="array" ref="Y9">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('m2pc BAU-S - starting point'!$C$2:$G$9,('m2pc BAU-S - starting point'!$A$2:$A$9='m2pc BAU-S'!$A9)),'m2pc BAU-S - starting point'!$C$1:$G$1='m2pc BAU-S'!Y$1),'m2pc BAU-S - starting point'!$B$2='m2pc BAU-S'!$B9)),0)</f>
-        <v>29.429221995017024</v>
+        <v>29.998060769980995</v>
       </c>
       <c r="Z9" s="6" cm="1">
         <f t="array" ref="Z9">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('m2pc BAU-S - starting point'!$C$2:$G$9,('m2pc BAU-S - starting point'!$A$2:$A$9='m2pc BAU-S'!$A9)),'m2pc BAU-S - starting point'!$C$1:$G$1='m2pc BAU-S'!Z$1),'m2pc BAU-S - starting point'!$B$2='m2pc BAU-S'!$B9)),0)</f>
-        <v>29.429221995017024</v>
+        <v>29.998060769980995</v>
       </c>
       <c r="AA9" s="6" cm="1">
         <f t="array" ref="AA9">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('m2pc BAU-S - starting point'!$C$2:$G$9,('m2pc BAU-S - starting point'!$A$2:$A$9='m2pc BAU-S'!$A9)),'m2pc BAU-S - starting point'!$C$1:$G$1='m2pc BAU-S'!AA$1),'m2pc BAU-S - starting point'!$B$2='m2pc BAU-S'!$B9)),0)</f>
-        <v>41.53798146111923</v>
+        <v>42.331809530047231</v>
       </c>
       <c r="AB9" s="6" cm="1">
         <f t="array" ref="AB9">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('m2pc BAU-S - starting point'!$C$2:$G$9,('m2pc BAU-S - starting point'!$A$2:$A$9='m2pc BAU-S'!$A9)),'m2pc BAU-S - starting point'!$C$1:$G$1='m2pc BAU-S'!AB$1),'m2pc BAU-S - starting point'!$B$2='m2pc BAU-S'!$B9)),0)</f>
-        <v>41.725351832173402</v>
+        <v>41.88202984670388</v>
       </c>
       <c r="AC9" s="6" cm="1">
         <f t="array" ref="AC9">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('m2pc BAU-S - starting point'!$C$2:$G$9,('m2pc BAU-S - starting point'!$A$2:$A$9='m2pc BAU-S'!$A9)),'m2pc BAU-S - starting point'!$C$1:$G$1='m2pc BAU-S'!AC$1),'m2pc BAU-S - starting point'!$B$2='m2pc BAU-S'!$B9)),0)</f>
-        <v>45.50824427817038</v>
+        <v>45.418860130202006</v>
       </c>
     </row>
     <row r="10" spans="1:29" x14ac:dyDescent="0.3">
@@ -6189,111 +6189,111 @@
       </c>
       <c r="C10" s="6" cm="1">
         <f t="array" ref="C10">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('m2pc BAU-S - starting point'!$C$2:$G$9,('m2pc BAU-S - starting point'!$A$2:$A$9='m2pc BAU-S'!$A10)),'m2pc BAU-S - starting point'!$C$1:$G$1='m2pc BAU-S'!C$1),'m2pc BAU-S - starting point'!$B$2='m2pc BAU-S'!$B10)),0)</f>
-        <v>45.50824427817038</v>
+        <v>44.551093593831069</v>
       </c>
       <c r="D10" s="6" cm="1">
         <f t="array" ref="D10">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('m2pc BAU-S - starting point'!$C$2:$G$9,('m2pc BAU-S - starting point'!$A$2:$A$9='m2pc BAU-S'!$A10)),'m2pc BAU-S - starting point'!$C$1:$G$1='m2pc BAU-S'!D$1),'m2pc BAU-S - starting point'!$B$2='m2pc BAU-S'!$B10)),0)</f>
-        <v>41.725351832173402</v>
+        <v>41.158125442575255</v>
       </c>
       <c r="E10" s="6" cm="1">
         <f t="array" ref="E10">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('m2pc BAU-S - starting point'!$C$2:$G$9,('m2pc BAU-S - starting point'!$A$2:$A$9='m2pc BAU-S'!$A10)),'m2pc BAU-S - starting point'!$C$1:$G$1='m2pc BAU-S'!E$1),'m2pc BAU-S - starting point'!$B$2='m2pc BAU-S'!$B10)),0)</f>
-        <v>29.429221995017024</v>
+        <v>29.598359919879897</v>
       </c>
       <c r="F10" s="6" cm="1">
         <f t="array" ref="F10">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('m2pc BAU-S - starting point'!$C$2:$G$9,('m2pc BAU-S - starting point'!$A$2:$A$9='m2pc BAU-S'!$A10)),'m2pc BAU-S - starting point'!$C$1:$G$1='m2pc BAU-S'!F$1),'m2pc BAU-S - starting point'!$B$2='m2pc BAU-S'!$B10)),0)</f>
-        <v>29.429221995017024</v>
+        <v>29.598359919879897</v>
       </c>
       <c r="G10" s="6" cm="1">
         <f t="array" ref="G10">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('m2pc BAU-S - starting point'!$C$2:$G$9,('m2pc BAU-S - starting point'!$A$2:$A$9='m2pc BAU-S'!$A10)),'m2pc BAU-S - starting point'!$C$1:$G$1='m2pc BAU-S'!G$1),'m2pc BAU-S - starting point'!$B$2='m2pc BAU-S'!$B10)),0)</f>
-        <v>54.261045846803263</v>
+        <v>52.796572524038808</v>
       </c>
       <c r="H10" s="6" cm="1">
         <f t="array" ref="H10">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('m2pc BAU-S - starting point'!$C$2:$G$9,('m2pc BAU-S - starting point'!$A$2:$A$9='m2pc BAU-S'!$A10)),'m2pc BAU-S - starting point'!$C$1:$G$1='m2pc BAU-S'!H$1),'m2pc BAU-S - starting point'!$B$2='m2pc BAU-S'!$B10)),0)</f>
-        <v>41.53798146111923</v>
+        <v>41.369009232557275</v>
       </c>
       <c r="I10" s="6" cm="1">
         <f t="array" ref="I10">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('m2pc BAU-S - starting point'!$C$2:$G$9,('m2pc BAU-S - starting point'!$A$2:$A$9='m2pc BAU-S'!$A10)),'m2pc BAU-S - starting point'!$C$1:$G$1='m2pc BAU-S'!I$1),'m2pc BAU-S - starting point'!$B$2='m2pc BAU-S'!$B10)),0)</f>
-        <v>54.261045846803263</v>
+        <v>52.796572524038808</v>
       </c>
       <c r="J10" s="6" cm="1">
         <f t="array" ref="J10">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('m2pc BAU-S - starting point'!$C$2:$G$9,('m2pc BAU-S - starting point'!$A$2:$A$9='m2pc BAU-S'!$A10)),'m2pc BAU-S - starting point'!$C$1:$G$1='m2pc BAU-S'!J$1),'m2pc BAU-S - starting point'!$B$2='m2pc BAU-S'!$B10)),0)</f>
-        <v>41.53798146111923</v>
+        <v>41.369009232557275</v>
       </c>
       <c r="K10" s="6" cm="1">
         <f t="array" ref="K10">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('m2pc BAU-S - starting point'!$C$2:$G$9,('m2pc BAU-S - starting point'!$A$2:$A$9='m2pc BAU-S'!$A10)),'m2pc BAU-S - starting point'!$C$1:$G$1='m2pc BAU-S'!K$1),'m2pc BAU-S - starting point'!$B$2='m2pc BAU-S'!$B10)),0)</f>
-        <v>41.725351832173402</v>
+        <v>41.158125442575255</v>
       </c>
       <c r="L10" s="6" cm="1">
         <f t="array" ref="L10">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('m2pc BAU-S - starting point'!$C$2:$G$9,('m2pc BAU-S - starting point'!$A$2:$A$9='m2pc BAU-S'!$A10)),'m2pc BAU-S - starting point'!$C$1:$G$1='m2pc BAU-S'!L$1),'m2pc BAU-S - starting point'!$B$2='m2pc BAU-S'!$B10)),0)</f>
-        <v>41.725351832173402</v>
+        <v>41.158125442575255</v>
       </c>
       <c r="M10" s="6" cm="1">
         <f t="array" ref="M10">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('m2pc BAU-S - starting point'!$C$2:$G$9,('m2pc BAU-S - starting point'!$A$2:$A$9='m2pc BAU-S'!$A10)),'m2pc BAU-S - starting point'!$C$1:$G$1='m2pc BAU-S'!M$1),'m2pc BAU-S - starting point'!$B$2='m2pc BAU-S'!$B10)),0)</f>
-        <v>45.50824427817038</v>
+        <v>44.551093593831069</v>
       </c>
       <c r="N10" s="6" cm="1">
         <f t="array" ref="N10">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('m2pc BAU-S - starting point'!$C$2:$G$9,('m2pc BAU-S - starting point'!$A$2:$A$9='m2pc BAU-S'!$A10)),'m2pc BAU-S - starting point'!$C$1:$G$1='m2pc BAU-S'!N$1),'m2pc BAU-S - starting point'!$B$2='m2pc BAU-S'!$B10)),0)</f>
-        <v>41.53798146111923</v>
+        <v>41.369009232557275</v>
       </c>
       <c r="O10" s="6" cm="1">
         <f t="array" ref="O10">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('m2pc BAU-S - starting point'!$C$2:$G$9,('m2pc BAU-S - starting point'!$A$2:$A$9='m2pc BAU-S'!$A10)),'m2pc BAU-S - starting point'!$C$1:$G$1='m2pc BAU-S'!O$1),'m2pc BAU-S - starting point'!$B$2='m2pc BAU-S'!$B10)),0)</f>
-        <v>41.53798146111923</v>
+        <v>41.369009232557275</v>
       </c>
       <c r="P10" s="6" cm="1">
         <f t="array" ref="P10">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('m2pc BAU-S - starting point'!$C$2:$G$9,('m2pc BAU-S - starting point'!$A$2:$A$9='m2pc BAU-S'!$A10)),'m2pc BAU-S - starting point'!$C$1:$G$1='m2pc BAU-S'!P$1),'m2pc BAU-S - starting point'!$B$2='m2pc BAU-S'!$B10)),0)</f>
-        <v>41.725351832173402</v>
+        <v>41.158125442575255</v>
       </c>
       <c r="Q10" s="6" cm="1">
         <f t="array" ref="Q10">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('m2pc BAU-S - starting point'!$C$2:$G$9,('m2pc BAU-S - starting point'!$A$2:$A$9='m2pc BAU-S'!$A10)),'m2pc BAU-S - starting point'!$C$1:$G$1='m2pc BAU-S'!Q$1),'m2pc BAU-S - starting point'!$B$2='m2pc BAU-S'!$B10)),0)</f>
-        <v>41.53798146111923</v>
+        <v>41.369009232557275</v>
       </c>
       <c r="R10" s="6" cm="1">
         <f t="array" ref="R10">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('m2pc BAU-S - starting point'!$C$2:$G$9,('m2pc BAU-S - starting point'!$A$2:$A$9='m2pc BAU-S'!$A10)),'m2pc BAU-S - starting point'!$C$1:$G$1='m2pc BAU-S'!R$1),'m2pc BAU-S - starting point'!$B$2='m2pc BAU-S'!$B10)),0)</f>
-        <v>29.429221995017024</v>
+        <v>29.598359919879897</v>
       </c>
       <c r="S10" s="6" cm="1">
         <f t="array" ref="S10">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('m2pc BAU-S - starting point'!$C$2:$G$9,('m2pc BAU-S - starting point'!$A$2:$A$9='m2pc BAU-S'!$A10)),'m2pc BAU-S - starting point'!$C$1:$G$1='m2pc BAU-S'!S$1),'m2pc BAU-S - starting point'!$B$2='m2pc BAU-S'!$B10)),0)</f>
-        <v>41.53798146111923</v>
+        <v>41.369009232557275</v>
       </c>
       <c r="T10" s="6" cm="1">
         <f t="array" ref="T10">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('m2pc BAU-S - starting point'!$C$2:$G$9,('m2pc BAU-S - starting point'!$A$2:$A$9='m2pc BAU-S'!$A10)),'m2pc BAU-S - starting point'!$C$1:$G$1='m2pc BAU-S'!T$1),'m2pc BAU-S - starting point'!$B$2='m2pc BAU-S'!$B10)),0)</f>
-        <v>54.261045846803263</v>
+        <v>52.796572524038808</v>
       </c>
       <c r="U10" s="6" cm="1">
         <f t="array" ref="U10">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('m2pc BAU-S - starting point'!$C$2:$G$9,('m2pc BAU-S - starting point'!$A$2:$A$9='m2pc BAU-S'!$A10)),'m2pc BAU-S - starting point'!$C$1:$G$1='m2pc BAU-S'!U$1),'m2pc BAU-S - starting point'!$B$2='m2pc BAU-S'!$B10)),0)</f>
-        <v>54.261045846803263</v>
+        <v>52.796572524038808</v>
       </c>
       <c r="V10" s="6" cm="1">
         <f t="array" ref="V10">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('m2pc BAU-S - starting point'!$C$2:$G$9,('m2pc BAU-S - starting point'!$A$2:$A$9='m2pc BAU-S'!$A10)),'m2pc BAU-S - starting point'!$C$1:$G$1='m2pc BAU-S'!V$1),'m2pc BAU-S - starting point'!$B$2='m2pc BAU-S'!$B10)),0)</f>
-        <v>54.261045846803263</v>
+        <v>52.796572524038808</v>
       </c>
       <c r="W10" s="6" cm="1">
         <f t="array" ref="W10">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('m2pc BAU-S - starting point'!$C$2:$G$9,('m2pc BAU-S - starting point'!$A$2:$A$9='m2pc BAU-S'!$A10)),'m2pc BAU-S - starting point'!$C$1:$G$1='m2pc BAU-S'!W$1),'m2pc BAU-S - starting point'!$B$2='m2pc BAU-S'!$B10)),0)</f>
-        <v>29.429221995017024</v>
+        <v>29.598359919879897</v>
       </c>
       <c r="X10" s="6" cm="1">
         <f t="array" ref="X10">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('m2pc BAU-S - starting point'!$C$2:$G$9,('m2pc BAU-S - starting point'!$A$2:$A$9='m2pc BAU-S'!$A10)),'m2pc BAU-S - starting point'!$C$1:$G$1='m2pc BAU-S'!X$1),'m2pc BAU-S - starting point'!$B$2='m2pc BAU-S'!$B10)),0)</f>
-        <v>45.50824427817038</v>
+        <v>44.551093593831069</v>
       </c>
       <c r="Y10" s="6" cm="1">
         <f t="array" ref="Y10">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('m2pc BAU-S - starting point'!$C$2:$G$9,('m2pc BAU-S - starting point'!$A$2:$A$9='m2pc BAU-S'!$A10)),'m2pc BAU-S - starting point'!$C$1:$G$1='m2pc BAU-S'!Y$1),'m2pc BAU-S - starting point'!$B$2='m2pc BAU-S'!$B10)),0)</f>
-        <v>29.429221995017024</v>
+        <v>29.598359919879897</v>
       </c>
       <c r="Z10" s="6" cm="1">
         <f t="array" ref="Z10">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('m2pc BAU-S - starting point'!$C$2:$G$9,('m2pc BAU-S - starting point'!$A$2:$A$9='m2pc BAU-S'!$A10)),'m2pc BAU-S - starting point'!$C$1:$G$1='m2pc BAU-S'!Z$1),'m2pc BAU-S - starting point'!$B$2='m2pc BAU-S'!$B10)),0)</f>
-        <v>29.429221995017024</v>
+        <v>29.598359919879897</v>
       </c>
       <c r="AA10" s="6" cm="1">
         <f t="array" ref="AA10">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('m2pc BAU-S - starting point'!$C$2:$G$9,('m2pc BAU-S - starting point'!$A$2:$A$9='m2pc BAU-S'!$A10)),'m2pc BAU-S - starting point'!$C$1:$G$1='m2pc BAU-S'!AA$1),'m2pc BAU-S - starting point'!$B$2='m2pc BAU-S'!$B10)),0)</f>
-        <v>41.53798146111923</v>
+        <v>41.369009232557275</v>
       </c>
       <c r="AB10" s="6" cm="1">
         <f t="array" ref="AB10">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('m2pc BAU-S - starting point'!$C$2:$G$9,('m2pc BAU-S - starting point'!$A$2:$A$9='m2pc BAU-S'!$A10)),'m2pc BAU-S - starting point'!$C$1:$G$1='m2pc BAU-S'!AB$1),'m2pc BAU-S - starting point'!$B$2='m2pc BAU-S'!$B10)),0)</f>
-        <v>41.725351832173402</v>
+        <v>41.158125442575255</v>
       </c>
       <c r="AC10" s="6" cm="1">
         <f t="array" ref="AC10">IFERROR(SUM(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('m2pc BAU-S - starting point'!$C$2:$G$9,('m2pc BAU-S - starting point'!$A$2:$A$9='m2pc BAU-S'!$A10)),'m2pc BAU-S - starting point'!$C$1:$G$1='m2pc BAU-S'!AC$1),'m2pc BAU-S - starting point'!$B$2='m2pc BAU-S'!$B10)),0)</f>
-        <v>45.50824427817038</v>
+        <v>44.551093593831069</v>
       </c>
     </row>
   </sheetData>
@@ -6302,6 +6302,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100241E96938535DD4B921FCDFB54345D30" ma:contentTypeVersion="18" ma:contentTypeDescription="Creare un nuovo documento." ma:contentTypeScope="" ma:versionID="a5d5c10fb5d76e91b5d3863d63e8b979">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="5d44ae6a-e145-4c9d-94e7-ddf9cc58067e" xmlns:ns3="e67e9a88-35e1-4b39-8da9-a609eb308282" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f7cec042378b2404c094b5ca61f00f7c" ns2:_="" ns3:_="">
     <xsd:import namespace="5d44ae6a-e145-4c9d-94e7-ddf9cc58067e"/>
@@ -6556,16 +6565,15 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8A1B00CF-E182-41C3-8348-7B2F8141874A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{52800BDC-EFD0-46DF-B0CE-306852B3E8C6}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6582,12 +6590,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8A1B00CF-E182-41C3-8348-7B2F8141874A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>